<commit_message>
traduction de la page 3807474e9e9f93a7da14ac36ad7ca915416ef0d6
</commit_message>
<xml_diff>
--- a/test-page/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
+++ b/test-page/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="451">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-16T07:42:16+00:00</t>
+    <t>2025-01-14T13:38:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1412,23 +1412,7 @@
     <t>Quantity actually administered to the patient or planned to be administered</t>
   </si>
   <si>
-    <t>The comparator is not used on a SimpleQuantity</t>
-  </si>
-  <si>
-    <t>The context of use may frequently define what kind of quantity this is and therefore what kind of units can be used. The context of use may also restrict the values for the comparator.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}</t>
-  </si>
-  <si>
     <t>quantiteAdministree</t>
-  </si>
-  <si>
-    <t>n/a,PQ, IVL&lt;PQ&gt;, MO, CO, depending on the values</t>
-  </si>
-  <si>
-    <t>SN (see also Range) or CQ</t>
   </si>
   <si>
     <t>MedicationAdministration.eventHistory</t>
@@ -9280,10 +9264,10 @@
         <v>443</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9342,13 +9326,13 @@
         <v>89</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>446</v>
+        <v>101</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>20</v>
@@ -9357,18 +9341,18 @@
         <v>20</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="AO65" t="s" s="2">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9391,16 +9375,16 @@
         <v>20</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -9450,7 +9434,7 @@
         <v>20</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>78</v>
@@ -9474,7 +9458,7 @@
         <v>20</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>20</v>

</xml_diff>